<commit_message>
many much moosen updates
</commit_message>
<xml_diff>
--- a/tests/data/Mathieu_2015_phi05_99_1atm.xlsx
+++ b/tests/data/Mathieu_2015_phi05_99_1atm.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mulvihcr/PycharmProjects/pythonProject/mechsimulator/tests/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6260B6D-9DCD-CD45-87DA-61581A4E4A63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAB6532E-50F2-3D49-82D0-D307FF3E3AE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12560" yWindow="2360" windowWidth="16960" windowHeight="12320" xr2:uid="{E8268F29-D532-4F4A-8DC7-DD2C0037AE91}"/>
+    <workbookView xWindow="14260" yWindow="2200" windowWidth="16960" windowHeight="12320" xr2:uid="{E8268F29-D532-4F4A-8DC7-DD2C0037AE91}"/>
   </bookViews>
   <sheets>
     <sheet name="info" sheetId="1" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="480" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="480" uniqueCount="59">
   <si>
     <t>parameter</t>
   </si>
@@ -137,9 +137,6 @@
     <t>atm</t>
   </si>
   <si>
-    <t>s</t>
-  </si>
-  <si>
     <t>X</t>
   </si>
   <si>
@@ -167,12 +164,6 @@
     <t>idt_method</t>
   </si>
   <si>
-    <t>OH*</t>
-  </si>
-  <si>
-    <t>idt_target</t>
-  </si>
-  <si>
     <t>[OH]</t>
   </si>
   <si>
@@ -225,6 +216,12 @@
   </si>
   <si>
     <t>ms</t>
+  </si>
+  <si>
+    <t>idt_targ</t>
+  </si>
+  <si>
+    <t>OHV</t>
   </si>
 </sst>
 </file>
@@ -617,7 +614,7 @@
   <dimension ref="A1:I28"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -629,7 +626,7 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B1" s="8" t="s">
         <v>0</v>
@@ -662,7 +659,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C3" s="9">
         <v>1</v>
@@ -679,10 +676,10 @@
         <v>4</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="D4" s="11" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E4" s="8"/>
       <c r="F4" s="8"/>
@@ -695,10 +692,10 @@
         <v>5</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E5" s="8"/>
       <c r="F5" s="8"/>
@@ -708,13 +705,13 @@
         <v>2</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C6" s="9" t="s">
         <v>26</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E6" s="8"/>
       <c r="F6" s="8"/>
@@ -724,13 +721,13 @@
         <v>2</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E7" s="8"/>
       <c r="F7" s="8"/>
@@ -746,7 +743,7 @@
         <v>11</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E8" s="8"/>
       <c r="F8" s="8"/>
@@ -763,7 +760,7 @@
         <v>14</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E9" s="8"/>
       <c r="F9" s="8"/>
@@ -840,10 +837,10 @@
         <v>24</v>
       </c>
       <c r="C14" s="9">
-        <v>3.0000000000000001E-3</v>
+        <v>10</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>30</v>
+        <v>56</v>
       </c>
       <c r="E14" s="8"/>
       <c r="F14" s="8"/>
@@ -853,10 +850,10 @@
         <v>7</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>41</v>
+        <v>57</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>40</v>
+        <v>58</v>
       </c>
       <c r="D15" s="8"/>
       <c r="E15" s="8"/>
@@ -869,10 +866,10 @@
         <v>7</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D16" s="8"/>
       <c r="E16" s="8"/>
@@ -882,10 +879,10 @@
     </row>
     <row r="17" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A17" s="8" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C17" s="9"/>
       <c r="D17" s="8"/>
@@ -897,13 +894,13 @@
         <v>20</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C18" s="10">
         <v>4.0000000000000001E-3</v>
       </c>
       <c r="D18" s="8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E18" s="8"/>
       <c r="F18" s="8"/>
@@ -913,13 +910,13 @@
         <v>20</v>
       </c>
       <c r="B19" s="8" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C19" s="10">
         <v>6.0000000000000001E-3</v>
       </c>
       <c r="D19" s="8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E19" s="8"/>
       <c r="F19" s="8"/>
@@ -935,7 +932,7 @@
         <v>0.99</v>
       </c>
       <c r="D20" s="8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E20" s="8"/>
       <c r="F20" s="8"/>
@@ -945,10 +942,10 @@
         <v>13</v>
       </c>
       <c r="B21" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="C21" s="12" t="s">
         <v>53</v>
-      </c>
-      <c r="C21" s="12" t="s">
-        <v>56</v>
       </c>
       <c r="D21" s="4">
         <v>1</v>
@@ -965,10 +962,10 @@
         <v>13</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C22" s="12" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="D22" s="4">
         <v>3</v>
@@ -1005,10 +1002,10 @@
         <v>13</v>
       </c>
       <c r="B24" s="8" t="s">
-        <v>40</v>
+        <v>58</v>
       </c>
       <c r="C24" s="9" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="D24" s="8">
         <v>2</v>
@@ -1022,33 +1019,33 @@
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
+        <v>40</v>
+      </c>
+      <c r="B25" t="s">
+        <v>41</v>
+      </c>
+      <c r="C25" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="D25" t="s">
         <v>43</v>
       </c>
-      <c r="B25" t="s">
+      <c r="E25" t="s">
         <v>44</v>
       </c>
-      <c r="C25" s="13" t="s">
+      <c r="F25" t="s">
         <v>45</v>
-      </c>
-      <c r="D25" t="s">
-        <v>46</v>
-      </c>
-      <c r="E25" t="s">
-        <v>47</v>
-      </c>
-      <c r="F25" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" s="4" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C26" s="9" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D26" s="8"/>
       <c r="E26" s="8"/>
@@ -1087,7 +1084,7 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -1180,7 +1177,7 @@
         <v>2500</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G5" s="4"/>
     </row>
@@ -1189,13 +1186,13 @@
         <v>20</v>
       </c>
       <c r="B6" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C6" s="1">
         <v>4.0000000000000001E-3</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E6">
         <v>1</v>
@@ -1212,13 +1209,13 @@
         <v>20</v>
       </c>
       <c r="B7" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C7" s="1">
         <v>6.0000000000000001E-3</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E7">
         <v>1</v>
@@ -1241,7 +1238,7 @@
         <v>0.998</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E8">
         <v>1</v>
@@ -1258,13 +1255,13 @@
         <v>21</v>
       </c>
       <c r="B9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C9" s="6">
         <v>170</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E9">
         <v>10</v>
@@ -1293,7 +1290,7 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -1386,7 +1383,7 @@
         <v>2500</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G5" s="4"/>
     </row>
@@ -1395,13 +1392,13 @@
         <v>20</v>
       </c>
       <c r="B6" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C6" s="1">
         <v>4.0000000000000001E-3</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E6">
         <v>1</v>
@@ -1418,13 +1415,13 @@
         <v>20</v>
       </c>
       <c r="B7" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C7" s="1">
         <v>6.0000000000000001E-3</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E7">
         <v>1</v>
@@ -1447,7 +1444,7 @@
         <v>0.998</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E8">
         <v>1</v>
@@ -1464,13 +1461,13 @@
         <v>21</v>
       </c>
       <c r="B9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C9" s="6">
         <v>129</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E9">
         <v>10</v>
@@ -1499,7 +1496,7 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -1592,7 +1589,7 @@
         <v>2500</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G5" s="4"/>
     </row>
@@ -1601,13 +1598,13 @@
         <v>20</v>
       </c>
       <c r="B6" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C6" s="1">
         <v>4.0000000000000001E-3</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E6">
         <v>1</v>
@@ -1624,13 +1621,13 @@
         <v>20</v>
       </c>
       <c r="B7" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C7" s="1">
         <v>6.0000000000000001E-3</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E7">
         <v>1</v>
@@ -1653,7 +1650,7 @@
         <v>0.998</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E8">
         <v>1</v>
@@ -1670,13 +1667,13 @@
         <v>21</v>
       </c>
       <c r="B9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C9" s="6">
         <v>91</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E9">
         <v>10</v>
@@ -1708,7 +1705,7 @@
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -1801,7 +1798,7 @@
         <v>2500</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G5" s="4"/>
     </row>
@@ -1810,13 +1807,13 @@
         <v>20</v>
       </c>
       <c r="B6" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C6" s="1">
         <v>4.0000000000000001E-3</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E6">
         <v>1</v>
@@ -1833,13 +1830,13 @@
         <v>20</v>
       </c>
       <c r="B7" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C7" s="1">
         <v>6.0000000000000001E-3</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E7">
         <v>1</v>
@@ -1862,7 +1859,7 @@
         <v>0.998</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E8">
         <v>1</v>
@@ -1879,13 +1876,13 @@
         <v>21</v>
       </c>
       <c r="B9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C9" s="6">
         <v>1113</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E9">
         <v>10</v>
@@ -1929,7 +1926,7 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -2022,7 +2019,7 @@
         <v>2500</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G5" s="4"/>
     </row>
@@ -2031,13 +2028,13 @@
         <v>20</v>
       </c>
       <c r="B6" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C6" s="1">
         <v>4.0000000000000001E-3</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E6">
         <v>1</v>
@@ -2054,13 +2051,13 @@
         <v>20</v>
       </c>
       <c r="B7" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C7" s="1">
         <v>6.0000000000000001E-3</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E7">
         <v>1</v>
@@ -2083,7 +2080,7 @@
         <v>0.998</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E8">
         <v>1</v>
@@ -2100,13 +2097,13 @@
         <v>21</v>
       </c>
       <c r="B9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C9" s="6">
         <v>998</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E9">
         <v>10</v>
@@ -2135,7 +2132,7 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -2228,7 +2225,7 @@
         <v>2500</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G5" s="4"/>
     </row>
@@ -2237,13 +2234,13 @@
         <v>20</v>
       </c>
       <c r="B6" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C6" s="1">
         <v>4.0000000000000001E-3</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E6">
         <v>1</v>
@@ -2260,13 +2257,13 @@
         <v>20</v>
       </c>
       <c r="B7" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C7" s="1">
         <v>6.0000000000000001E-3</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E7">
         <v>1</v>
@@ -2289,7 +2286,7 @@
         <v>0.998</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E8">
         <v>1</v>
@@ -2306,13 +2303,13 @@
         <v>21</v>
       </c>
       <c r="B9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C9" s="6">
         <v>783</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E9">
         <v>10</v>
@@ -2341,7 +2338,7 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -2434,7 +2431,7 @@
         <v>2500</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G5" s="4"/>
     </row>
@@ -2443,13 +2440,13 @@
         <v>20</v>
       </c>
       <c r="B6" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C6" s="1">
         <v>4.0000000000000001E-3</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E6">
         <v>1</v>
@@ -2466,13 +2463,13 @@
         <v>20</v>
       </c>
       <c r="B7" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C7" s="1">
         <v>6.0000000000000001E-3</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E7">
         <v>1</v>
@@ -2495,7 +2492,7 @@
         <v>0.998</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E8">
         <v>1</v>
@@ -2512,13 +2509,13 @@
         <v>21</v>
       </c>
       <c r="B9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C9" s="6">
         <v>769</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E9">
         <v>10</v>
@@ -2547,7 +2544,7 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -2640,7 +2637,7 @@
         <v>2500</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G5" s="4"/>
     </row>
@@ -2649,13 +2646,13 @@
         <v>20</v>
       </c>
       <c r="B6" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C6" s="1">
         <v>4.0000000000000001E-3</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E6">
         <v>1</v>
@@ -2672,13 +2669,13 @@
         <v>20</v>
       </c>
       <c r="B7" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C7" s="1">
         <v>6.0000000000000001E-3</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E7">
         <v>1</v>
@@ -2701,7 +2698,7 @@
         <v>0.998</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E8">
         <v>1</v>
@@ -2718,13 +2715,13 @@
         <v>21</v>
       </c>
       <c r="B9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C9" s="6">
         <v>551</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E9">
         <v>10</v>
@@ -2753,7 +2750,7 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -2846,7 +2843,7 @@
         <v>2500</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G5" s="4"/>
     </row>
@@ -2855,13 +2852,13 @@
         <v>20</v>
       </c>
       <c r="B6" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C6" s="1">
         <v>4.0000000000000001E-3</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E6">
         <v>1</v>
@@ -2878,13 +2875,13 @@
         <v>20</v>
       </c>
       <c r="B7" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C7" s="1">
         <v>6.0000000000000001E-3</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E7">
         <v>1</v>
@@ -2907,7 +2904,7 @@
         <v>0.998</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E8">
         <v>1</v>
@@ -2924,13 +2921,13 @@
         <v>21</v>
       </c>
       <c r="B9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C9" s="6">
         <v>380</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E9">
         <v>10</v>
@@ -2959,7 +2956,7 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -3052,7 +3049,7 @@
         <v>2500</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G5" s="4"/>
     </row>
@@ -3061,13 +3058,13 @@
         <v>20</v>
       </c>
       <c r="B6" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C6" s="1">
         <v>4.0000000000000001E-3</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E6">
         <v>1</v>
@@ -3084,13 +3081,13 @@
         <v>20</v>
       </c>
       <c r="B7" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C7" s="1">
         <v>6.0000000000000001E-3</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E7">
         <v>1</v>
@@ -3113,7 +3110,7 @@
         <v>0.998</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E8">
         <v>1</v>
@@ -3130,13 +3127,13 @@
         <v>21</v>
       </c>
       <c r="B9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C9" s="6">
         <v>362</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E9">
         <v>10</v>
@@ -3165,7 +3162,7 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -3258,7 +3255,7 @@
         <v>2500</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G5" s="4"/>
     </row>
@@ -3267,13 +3264,13 @@
         <v>20</v>
       </c>
       <c r="B6" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C6" s="1">
         <v>4.0000000000000001E-3</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E6">
         <v>1</v>
@@ -3290,13 +3287,13 @@
         <v>20</v>
       </c>
       <c r="B7" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C7" s="1">
         <v>6.0000000000000001E-3</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E7">
         <v>1</v>
@@ -3319,7 +3316,7 @@
         <v>0.998</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E8">
         <v>1</v>
@@ -3336,13 +3333,13 @@
         <v>21</v>
       </c>
       <c r="B9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C9" s="6">
         <v>226</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E9">
         <v>10</v>

</xml_diff>